<commit_message>
changes to deal with a problem I had running code on one of Ching-Ho's alignments (test4)
</commit_message>
<xml_diff>
--- a/test_data/test_rareVariants/test1/test1.MK.xlsx
+++ b/test_data/test_rareVariants/test1/test1.MK.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t xml:space="preserve">input</t>
   </si>
@@ -186,10 +186,22 @@
     <t xml:space="preserve">pop2 rare flags</t>
   </si>
   <si>
+    <t xml:space="preserve">pop1 codon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pop1 codonPos</t>
+  </si>
+  <si>
     <t xml:space="preserve">pop1 Pn</t>
   </si>
   <si>
     <t xml:space="preserve">pop1 Ps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pop2 codon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pop2 codonPos</t>
   </si>
   <si>
     <t xml:space="preserve">pop2 Pn</t>
@@ -207,10 +219,16 @@
     <t xml:space="preserve">T</t>
   </si>
   <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
     <t xml:space="preserve">G</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">0.7</t>
@@ -228,7 +246,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
@@ -628,10 +646,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="1">
+    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="true">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
     </sheetView>
   </sheetViews>
@@ -784,10 +802,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="120" showGridLines="1" tabSelected="false">
       <pane ySplit="1" xSplit="3" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -828,10 +846,14 @@
     <col min="32" max="32" width="18.39125" hidden="0" customWidth="1"/>
     <col min="33" max="33" width="18.39125" hidden="0" customWidth="1"/>
     <col min="34" max="34" width="18.39125" hidden="0" customWidth="1"/>
-    <col min="35" max="35" width="8.96125" hidden="0" customWidth="1"/>
-    <col min="36" max="36" width="8.96125" hidden="0" customWidth="1"/>
+    <col min="35" max="35" width="12.4975" hidden="0" customWidth="1"/>
+    <col min="36" max="36" width="16.03375" hidden="0" customWidth="1"/>
     <col min="37" max="37" width="8.96125" hidden="0" customWidth="1"/>
     <col min="38" max="38" width="8.96125" hidden="0" customWidth="1"/>
+    <col min="39" max="39" width="12.4975" hidden="0" customWidth="1"/>
+    <col min="40" max="40" width="16.03375" hidden="0" customWidth="1"/>
+    <col min="41" max="41" width="8.96125" hidden="0" customWidth="1"/>
+    <col min="42" max="42" width="8.96125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="150" customHeight="1">
@@ -949,6 +971,18 @@
       <c r="AL1" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="AM1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="n">
@@ -961,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E2" s="18" t="b">
         <v>0</v>
@@ -970,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H2" s="18" t="b">
         <v>0</v>
@@ -1000,11 +1034,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R2" s="18"/>
       <c r="S2" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
@@ -1027,11 +1061,11 @@
         <v>0</v>
       </c>
       <c r="AB2" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AC2" s="18"/>
       <c r="AD2" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE2" s="18"/>
       <c r="AF2" s="18"/>
@@ -1042,10 +1076,10 @@
         <v>0</v>
       </c>
       <c r="AI2" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="18" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="AK2" s="18" t="n">
         <v>0</v>
@@ -1053,7 +1087,19 @@
       <c r="AL2" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="AM2" s="22"/>
+      <c r="AM2" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO2" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="22"/>
     </row>
     <row r="3">
       <c r="A3" s="18" t="n">
@@ -1066,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E3" s="18" t="b">
         <v>0</v>
@@ -1075,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H3" s="18" t="b">
         <v>0</v>
@@ -1105,11 +1151,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R3" s="18"/>
       <c r="S3" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
@@ -1132,21 +1178,21 @@
         <v>0</v>
       </c>
       <c r="AB3" s="18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC3" s="18"/>
       <c r="AD3" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE3" s="18"/>
       <c r="AF3" s="18"/>
       <c r="AG3" s="19"/>
       <c r="AH3" s="18"/>
       <c r="AI3" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="18" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="AK3" s="18" t="n">
         <v>0</v>
@@ -1154,7 +1200,19 @@
       <c r="AL3" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="AM3" s="22"/>
+      <c r="AM3" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO3" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="22"/>
     </row>
     <row r="4">
       <c r="A4" s="20" t="n">
@@ -1167,7 +1225,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E4" s="20" t="b">
         <v>0</v>
@@ -1176,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H4" s="20" t="b">
         <v>0</v>
@@ -1206,11 +1264,11 @@
         <v>0</v>
       </c>
       <c r="Q4" s="20" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R4" s="20"/>
       <c r="S4" s="20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T4" s="20"/>
       <c r="U4" s="20"/>
@@ -1233,21 +1291,21 @@
         <v>0</v>
       </c>
       <c r="AB4" s="20" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC4" s="20"/>
       <c r="AD4" s="20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE4" s="20"/>
       <c r="AF4" s="20"/>
       <c r="AG4" s="21"/>
       <c r="AH4" s="20"/>
       <c r="AI4" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="20" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="AK4" s="20" t="n">
         <v>0</v>
@@ -1255,7 +1313,19 @@
       <c r="AL4" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AM4" s="22"/>
+      <c r="AM4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="22"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="n">
@@ -1268,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E5" s="13" t="b">
         <v>0</v>
@@ -1277,7 +1347,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H5" s="13" t="b">
         <v>0</v>
@@ -1307,11 +1377,11 @@
         <v>0</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R5" s="13"/>
       <c r="S5" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T5" s="13"/>
       <c r="U5" s="13"/>
@@ -1334,11 +1404,11 @@
         <v>0</v>
       </c>
       <c r="AB5" s="13" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC5" s="13"/>
       <c r="AD5" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE5" s="13"/>
       <c r="AF5" s="13"/>
@@ -1349,10 +1419,10 @@
         <v>0</v>
       </c>
       <c r="AI5" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="13" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="AK5" s="13" t="n">
         <v>0</v>
@@ -1360,7 +1430,19 @@
       <c r="AL5" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="AM5" s="17"/>
+      <c r="AM5" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO5" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="17"/>
     </row>
     <row r="6">
       <c r="A6" s="13" t="n">
@@ -1373,7 +1455,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E6" s="13" t="b">
         <v>0</v>
@@ -1382,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H6" s="13" t="b">
         <v>0</v>
@@ -1412,11 +1494,11 @@
         <v>0</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R6" s="13"/>
       <c r="S6" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
@@ -1439,21 +1521,21 @@
         <v>0</v>
       </c>
       <c r="AB6" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AC6" s="13"/>
       <c r="AD6" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE6" s="13"/>
       <c r="AF6" s="13"/>
       <c r="AG6" s="14"/>
       <c r="AH6" s="13"/>
       <c r="AI6" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="13" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="AK6" s="13" t="n">
         <v>0</v>
@@ -1461,7 +1543,19 @@
       <c r="AL6" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="AM6" s="17"/>
+      <c r="AM6" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO6" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="17"/>
     </row>
     <row r="7">
       <c r="A7" s="15" t="n">
@@ -1474,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E7" s="15" t="b">
         <v>1</v>
@@ -1483,7 +1577,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H7" s="15" t="b">
         <v>0</v>
@@ -1513,62 +1607,74 @@
         <v>0</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="T7" s="15" t="n">
         <v>0.3</v>
       </c>
       <c r="U7" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="V7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="V7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="15" t="s">
-        <v>63</v>
       </c>
       <c r="AC7" s="15"/>
       <c r="AD7" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE7" s="15"/>
       <c r="AF7" s="15"/>
       <c r="AG7" s="16"/>
       <c r="AH7" s="15"/>
       <c r="AI7" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="15" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="AK7" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL7" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="AM7" s="17"/>
+      <c r="AM7" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN7" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="17"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1581,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
@@ -1590,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H8" s="2" t="b">
         <v>0</v>
@@ -1620,11 +1726,11 @@
         <v>0</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -1647,11 +1753,11 @@
         <v>0</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
@@ -1662,15 +1768,27 @@
         <v>0</v>
       </c>
       <c r="AI8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1685,7 +1803,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -1694,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H9" s="2" t="b">
         <v>0</v>
@@ -1724,11 +1842,11 @@
         <v>0</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -1751,26 +1869,38 @@
         <v>0</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="4"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1785,7 +1915,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E10" s="11" t="b">
         <v>0</v>
@@ -1794,7 +1924,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H10" s="11" t="b">
         <v>0</v>
@@ -1824,11 +1954,11 @@
         <v>0</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R10" s="11"/>
       <c r="S10" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T10" s="11"/>
       <c r="U10" s="11"/>
@@ -1851,26 +1981,38 @@
         <v>0</v>
       </c>
       <c r="AB10" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC10" s="11"/>
       <c r="AD10" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="12"/>
       <c r="AH10" s="11"/>
       <c r="AI10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="11" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1885,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
@@ -1894,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H11" s="2" t="b">
         <v>0</v>
@@ -1924,11 +2066,11 @@
         <v>0</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -1951,11 +2093,11 @@
         <v>0</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
@@ -1966,15 +2108,27 @@
         <v>0</v>
       </c>
       <c r="AI11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1989,7 +2143,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
@@ -1998,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H12" s="2" t="b">
         <v>0</v>
@@ -2028,11 +2182,11 @@
         <v>0</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
@@ -2055,26 +2209,38 @@
         <v>0</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="4"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2089,7 +2255,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E13" s="11" t="b">
         <v>0</v>
@@ -2098,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H13" s="11" t="b">
         <v>0</v>
@@ -2128,11 +2294,11 @@
         <v>0</v>
       </c>
       <c r="Q13" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R13" s="11"/>
       <c r="S13" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T13" s="11"/>
       <c r="U13" s="11"/>
@@ -2155,26 +2321,38 @@
         <v>0</v>
       </c>
       <c r="AB13" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC13" s="11"/>
       <c r="AD13" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE13" s="11"/>
       <c r="AF13" s="11"/>
       <c r="AG13" s="12"/>
       <c r="AH13" s="11"/>
       <c r="AI13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="11" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="AJ13" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2189,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
@@ -2198,7 +2376,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H14" s="2" t="b">
         <v>0</v>
@@ -2228,11 +2406,11 @@
         <v>0</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
@@ -2255,11 +2433,11 @@
         <v>0</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
@@ -2270,15 +2448,27 @@
         <v>0</v>
       </c>
       <c r="AI14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="2" t="n">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2293,7 +2483,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -2302,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H15" s="2" t="b">
         <v>0</v>
@@ -2332,11 +2522,11 @@
         <v>0</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
@@ -2359,26 +2549,38 @@
         <v>0</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="4"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="2" t="n">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2393,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E16" s="11" t="b">
         <v>0</v>
@@ -2402,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H16" s="11" t="b">
         <v>0</v>
@@ -2432,19 +2634,19 @@
         <v>0</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="T16" s="11" t="n">
         <v>0.1</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="V16" s="12" t="n">
         <v>0</v>
@@ -2465,26 +2667,38 @@
         <v>0</v>
       </c>
       <c r="AB16" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC16" s="11"/>
       <c r="AD16" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE16" s="11"/>
       <c r="AF16" s="11"/>
       <c r="AG16" s="12"/>
       <c r="AH16" s="11"/>
       <c r="AI16" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="11" t="n">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AJ16" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK16" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL16" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN16" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO16" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2499,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2" t="b">
         <v>0</v>
@@ -2508,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H17" s="2" t="b">
         <v>0</v>
@@ -2538,11 +2752,11 @@
         <v>0</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
@@ -2565,11 +2779,11 @@
         <v>0</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
@@ -2580,15 +2794,27 @@
         <v>0</v>
       </c>
       <c r="AI17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="2" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2603,7 +2829,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="b">
         <v>0</v>
@@ -2612,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H18" s="2" t="b">
         <v>0</v>
@@ -2642,11 +2868,11 @@
         <v>0</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
@@ -2669,26 +2895,38 @@
         <v>0</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="4"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="2" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2703,7 +2941,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E19" s="11" t="b">
         <v>0</v>
@@ -2712,7 +2950,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H19" s="11" t="b">
         <v>0</v>
@@ -2742,11 +2980,11 @@
         <v>0</v>
       </c>
       <c r="Q19" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R19" s="11"/>
       <c r="S19" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
@@ -2769,26 +3007,38 @@
         <v>0</v>
       </c>
       <c r="AB19" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AC19" s="11"/>
       <c r="AD19" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE19" s="11"/>
       <c r="AF19" s="11"/>
       <c r="AG19" s="12"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="AJ19" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK19" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL19" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO19" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2803,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E20" s="2" t="b">
         <v>0</v>
@@ -2812,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H20" s="2" t="b">
         <v>0</v>
@@ -2842,11 +3092,11 @@
         <v>0</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -2869,11 +3119,11 @@
         <v>0</v>
       </c>
       <c r="AB20" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
@@ -2884,15 +3134,27 @@
         <v>0</v>
       </c>
       <c r="AI20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="2" t="n">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AN20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2907,7 +3169,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E21" s="2" t="b">
         <v>0</v>
@@ -2916,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H21" s="2" t="b">
         <v>0</v>
@@ -2946,11 +3208,11 @@
         <v>0</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
@@ -2973,26 +3235,38 @@
         <v>0</v>
       </c>
       <c r="AB21" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ21" s="2" t="n">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="AJ21" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AN21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3007,7 +3281,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E22" s="11" t="b">
         <v>0</v>
@@ -3016,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H22" s="11" t="b">
         <v>0</v>
@@ -3046,11 +3320,11 @@
         <v>0</v>
       </c>
       <c r="Q22" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R22" s="11"/>
       <c r="S22" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T22" s="11"/>
       <c r="U22" s="11"/>
@@ -3073,26 +3347,38 @@
         <v>0</v>
       </c>
       <c r="AB22" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC22" s="11"/>
       <c r="AD22" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE22" s="11"/>
       <c r="AF22" s="11"/>
       <c r="AG22" s="12"/>
       <c r="AH22" s="11"/>
       <c r="AI22" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="11" t="n">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="AJ22" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK22" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL22" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AN22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO22" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP22" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3107,7 +3393,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E23" s="2" t="b">
         <v>0</v>
@@ -3116,7 +3402,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H23" s="2" t="b">
         <v>0</v>
@@ -3146,11 +3432,11 @@
         <v>0</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
@@ -3173,11 +3459,11 @@
         <v>0</v>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
@@ -3188,15 +3474,27 @@
         <v>0</v>
       </c>
       <c r="AI23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="2" t="n">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="AJ23" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="AN23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP23" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3211,7 +3509,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E24" s="2" t="b">
         <v>0</v>
@@ -3220,7 +3518,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H24" s="2" t="b">
         <v>0</v>
@@ -3250,11 +3548,11 @@
         <v>0</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
@@ -3277,26 +3575,38 @@
         <v>0</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC24" s="2"/>
       <c r="AD24" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE24" s="2"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="4"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="2" t="n">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="AJ24" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="AN24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP24" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3311,7 +3621,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E25" s="11" t="b">
         <v>0</v>
@@ -3320,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H25" s="11" t="b">
         <v>0</v>
@@ -3350,11 +3660,11 @@
         <v>0</v>
       </c>
       <c r="Q25" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R25" s="11"/>
       <c r="S25" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
@@ -3377,26 +3687,38 @@
         <v>0</v>
       </c>
       <c r="AB25" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC25" s="11"/>
       <c r="AD25" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE25" s="11"/>
       <c r="AF25" s="11"/>
       <c r="AG25" s="12"/>
       <c r="AH25" s="11"/>
       <c r="AI25" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ25" s="11" t="n">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="AJ25" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK25" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="AN25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP25" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3411,7 +3733,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E26" s="2" t="b">
         <v>0</v>
@@ -3420,7 +3742,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H26" s="2" t="b">
         <v>0</v>
@@ -3450,11 +3772,11 @@
         <v>0</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
@@ -3477,11 +3799,11 @@
         <v>0</v>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
@@ -3492,15 +3814,27 @@
         <v>0</v>
       </c>
       <c r="AI26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="2" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="AJ26" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="AN26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3515,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E27" s="2" t="b">
         <v>0</v>
@@ -3524,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H27" s="2" t="b">
         <v>0</v>
@@ -3554,11 +3888,11 @@
         <v>0</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
@@ -3581,26 +3915,38 @@
         <v>0</v>
       </c>
       <c r="AB27" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="4"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ27" s="2" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="AN27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3615,7 +3961,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E28" s="11" t="b">
         <v>0</v>
@@ -3624,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H28" s="11" t="b">
         <v>0</v>
@@ -3654,11 +4000,11 @@
         <v>0</v>
       </c>
       <c r="Q28" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R28" s="11"/>
       <c r="S28" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T28" s="11"/>
       <c r="U28" s="11"/>
@@ -3681,26 +4027,38 @@
         <v>0</v>
       </c>
       <c r="AB28" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC28" s="11"/>
       <c r="AD28" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE28" s="11"/>
       <c r="AF28" s="11"/>
       <c r="AG28" s="12"/>
       <c r="AH28" s="11"/>
       <c r="AI28" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ28" s="11" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="AJ28" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK28" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL28" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="AN28" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO28" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP28" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3715,7 +4073,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E29" s="2" t="b">
         <v>0</v>
@@ -3724,7 +4082,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H29" s="2" t="b">
         <v>0</v>
@@ -3754,11 +4112,11 @@
         <v>0</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
@@ -3781,11 +4139,11 @@
         <v>0</v>
       </c>
       <c r="AB29" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
@@ -3796,15 +4154,27 @@
         <v>0</v>
       </c>
       <c r="AI29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ29" s="2" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AJ29" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AN29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP29" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3819,7 +4189,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E30" s="2" t="b">
         <v>0</v>
@@ -3828,7 +4198,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H30" s="2" t="b">
         <v>0</v>
@@ -3858,11 +4228,11 @@
         <v>0</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -3885,26 +4255,38 @@
         <v>0</v>
       </c>
       <c r="AB30" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC30" s="2"/>
       <c r="AD30" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="4"/>
       <c r="AH30" s="2"/>
       <c r="AI30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="2" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AJ30" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AN30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP30" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3919,7 +4301,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E31" s="11" t="b">
         <v>0</v>
@@ -3928,7 +4310,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H31" s="11" t="b">
         <v>0</v>
@@ -3958,11 +4340,11 @@
         <v>0</v>
       </c>
       <c r="Q31" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R31" s="11"/>
       <c r="S31" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T31" s="11"/>
       <c r="U31" s="11"/>
@@ -3985,26 +4367,38 @@
         <v>0</v>
       </c>
       <c r="AB31" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC31" s="11"/>
       <c r="AD31" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE31" s="11"/>
       <c r="AF31" s="11"/>
       <c r="AG31" s="12"/>
       <c r="AH31" s="11"/>
       <c r="AI31" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ31" s="11" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AJ31" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK31" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL31" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AN31" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO31" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP31" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4019,7 +4413,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E32" s="2" t="b">
         <v>0</v>
@@ -4028,7 +4422,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H32" s="2" t="b">
         <v>0</v>
@@ -4058,11 +4452,11 @@
         <v>0</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
@@ -4085,11 +4479,11 @@
         <v>0</v>
       </c>
       <c r="AB32" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC32" s="2"/>
       <c r="AD32" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
@@ -4100,15 +4494,27 @@
         <v>0</v>
       </c>
       <c r="AI32" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ32" s="2" t="n">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="AJ32" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AN32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP32" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4123,7 +4529,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E33" s="2" t="b">
         <v>0</v>
@@ -4132,7 +4538,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H33" s="2" t="b">
         <v>0</v>
@@ -4162,11 +4568,11 @@
         <v>0</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
@@ -4189,26 +4595,38 @@
         <v>0</v>
       </c>
       <c r="AB33" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE33" s="2"/>
       <c r="AF33" s="2"/>
       <c r="AG33" s="4"/>
       <c r="AH33" s="2"/>
       <c r="AI33" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ33" s="2" t="n">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="AJ33" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AN33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP33" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4223,7 +4641,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E34" s="11" t="b">
         <v>0</v>
@@ -4232,7 +4650,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H34" s="11" t="b">
         <v>0</v>
@@ -4262,11 +4680,11 @@
         <v>0</v>
       </c>
       <c r="Q34" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R34" s="11"/>
       <c r="S34" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T34" s="11"/>
       <c r="U34" s="11"/>
@@ -4289,26 +4707,38 @@
         <v>0</v>
       </c>
       <c r="AB34" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC34" s="11"/>
       <c r="AD34" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE34" s="11"/>
       <c r="AF34" s="11"/>
       <c r="AG34" s="12"/>
       <c r="AH34" s="11"/>
       <c r="AI34" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ34" s="11" t="n">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="AJ34" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK34" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL34" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="AN34" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO34" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP34" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4323,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E35" s="2" t="b">
         <v>0</v>
@@ -4332,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H35" s="2" t="b">
         <v>0</v>
@@ -4362,11 +4792,11 @@
         <v>0</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R35" s="2"/>
       <c r="S35" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
@@ -4389,11 +4819,11 @@
         <v>0</v>
       </c>
       <c r="AB35" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC35" s="2"/>
       <c r="AD35" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE35" s="2"/>
       <c r="AF35" s="2"/>
@@ -4404,15 +4834,27 @@
         <v>0</v>
       </c>
       <c r="AI35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ35" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AJ35" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM35" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="AN35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP35" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4427,7 +4869,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E36" s="2" t="b">
         <v>0</v>
@@ -4436,7 +4878,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H36" s="2" t="b">
         <v>0</v>
@@ -4466,11 +4908,11 @@
         <v>0</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R36" s="2"/>
       <c r="S36" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
@@ -4493,26 +4935,38 @@
         <v>0</v>
       </c>
       <c r="AB36" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC36" s="2"/>
       <c r="AD36" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="4"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ36" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AJ36" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="AN36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP36" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4527,7 +4981,7 @@
         <v>3</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E37" s="11" t="b">
         <v>0</v>
@@ -4536,7 +4990,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H37" s="11" t="b">
         <v>0</v>
@@ -4566,11 +5020,11 @@
         <v>0</v>
       </c>
       <c r="Q37" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R37" s="11"/>
       <c r="S37" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T37" s="11"/>
       <c r="U37" s="11"/>
@@ -4593,26 +5047,38 @@
         <v>0</v>
       </c>
       <c r="AB37" s="11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC37" s="11"/>
       <c r="AD37" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE37" s="11"/>
       <c r="AF37" s="11"/>
       <c r="AG37" s="12"/>
       <c r="AH37" s="11"/>
       <c r="AI37" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ37" s="11" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="AJ37" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK37" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL37" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM37" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="AN37" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO37" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP37" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4627,7 +5093,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E38" s="2" t="b">
         <v>0</v>
@@ -4636,7 +5102,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H38" s="2" t="b">
         <v>0</v>
@@ -4666,11 +5132,11 @@
         <v>0</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R38" s="2"/>
       <c r="S38" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
@@ -4693,11 +5159,11 @@
         <v>0</v>
       </c>
       <c r="AB38" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC38" s="2"/>
       <c r="AD38" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE38" s="2"/>
       <c r="AF38" s="2"/>
@@ -4708,15 +5174,27 @@
         <v>0</v>
       </c>
       <c r="AI38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ38" s="2" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="AJ38" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="AN38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP38" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4731,7 +5209,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E39" s="2" t="b">
         <v>0</v>
@@ -4740,7 +5218,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H39" s="2" t="b">
         <v>0</v>
@@ -4770,11 +5248,11 @@
         <v>0</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R39" s="2"/>
       <c r="S39" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
@@ -4797,26 +5275,38 @@
         <v>0</v>
       </c>
       <c r="AB39" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC39" s="2"/>
       <c r="AD39" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE39" s="2"/>
       <c r="AF39" s="2"/>
       <c r="AG39" s="4"/>
       <c r="AH39" s="2"/>
       <c r="AI39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ39" s="2" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="AJ39" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK39" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM39" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="AN39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP39" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4831,7 +5321,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E40" s="11" t="b">
         <v>0</v>
@@ -4840,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H40" s="11" t="b">
         <v>0</v>
@@ -4870,11 +5360,11 @@
         <v>0</v>
       </c>
       <c r="Q40" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R40" s="11"/>
       <c r="S40" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T40" s="11"/>
       <c r="U40" s="11"/>
@@ -4897,26 +5387,38 @@
         <v>0</v>
       </c>
       <c r="AB40" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC40" s="11"/>
       <c r="AD40" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE40" s="11"/>
       <c r="AF40" s="11"/>
       <c r="AG40" s="12"/>
       <c r="AH40" s="11"/>
       <c r="AI40" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ40" s="11" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="AJ40" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK40" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL40" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="AN40" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO40" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP40" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4931,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E41" s="2" t="b">
         <v>0</v>
@@ -4940,7 +5442,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H41" s="2" t="b">
         <v>0</v>
@@ -4970,11 +5472,11 @@
         <v>0</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R41" s="2"/>
       <c r="S41" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
@@ -4997,11 +5499,11 @@
         <v>0</v>
       </c>
       <c r="AB41" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
@@ -5012,15 +5514,27 @@
         <v>0</v>
       </c>
       <c r="AI41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ41" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="AJ41" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM41" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="AN41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP41" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5035,7 +5549,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E42" s="2" t="b">
         <v>0</v>
@@ -5044,7 +5558,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H42" s="2" t="b">
         <v>0</v>
@@ -5074,11 +5588,11 @@
         <v>0</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
@@ -5101,26 +5615,38 @@
         <v>0</v>
       </c>
       <c r="AB42" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC42" s="2"/>
       <c r="AD42" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="4"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ42" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="AJ42" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK42" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM42" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="AN42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP42" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5135,7 +5661,7 @@
         <v>3</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E43" s="11" t="b">
         <v>0</v>
@@ -5144,7 +5670,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H43" s="11" t="b">
         <v>0</v>
@@ -5174,11 +5700,11 @@
         <v>0</v>
       </c>
       <c r="Q43" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R43" s="11"/>
       <c r="S43" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T43" s="11"/>
       <c r="U43" s="11"/>
@@ -5201,26 +5727,38 @@
         <v>0</v>
       </c>
       <c r="AB43" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC43" s="11"/>
       <c r="AD43" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE43" s="11"/>
       <c r="AF43" s="11"/>
       <c r="AG43" s="12"/>
       <c r="AH43" s="11"/>
       <c r="AI43" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ43" s="11" t="n">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="AJ43" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK43" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL43" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM43" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="AN43" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO43" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP43" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5235,7 +5773,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E44" s="2" t="b">
         <v>0</v>
@@ -5244,7 +5782,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H44" s="2" t="b">
         <v>0</v>
@@ -5274,11 +5812,11 @@
         <v>0</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R44" s="2"/>
       <c r="S44" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
@@ -5301,11 +5839,11 @@
         <v>0</v>
       </c>
       <c r="AB44" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC44" s="2"/>
       <c r="AD44" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE44" s="2"/>
       <c r="AF44" s="2"/>
@@ -5316,15 +5854,27 @@
         <v>0</v>
       </c>
       <c r="AI44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ44" s="2" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="AJ44" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK44" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM44" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="AN44" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP44" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5339,7 +5889,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E45" s="2" t="b">
         <v>0</v>
@@ -5348,7 +5898,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H45" s="2" t="b">
         <v>0</v>
@@ -5378,11 +5928,11 @@
         <v>0</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
@@ -5405,26 +5955,38 @@
         <v>0</v>
       </c>
       <c r="AB45" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE45" s="2"/>
       <c r="AF45" s="2"/>
       <c r="AG45" s="4"/>
       <c r="AH45" s="2"/>
       <c r="AI45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ45" s="2" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="AJ45" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK45" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM45" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="AN45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP45" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5439,7 +6001,7 @@
         <v>3</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E46" s="11" t="b">
         <v>0</v>
@@ -5448,7 +6010,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H46" s="11" t="b">
         <v>0</v>
@@ -5478,11 +6040,11 @@
         <v>0</v>
       </c>
       <c r="Q46" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R46" s="11"/>
       <c r="S46" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T46" s="11"/>
       <c r="U46" s="11"/>
@@ -5505,26 +6067,38 @@
         <v>0</v>
       </c>
       <c r="AB46" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC46" s="11"/>
       <c r="AD46" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE46" s="11"/>
       <c r="AF46" s="11"/>
       <c r="AG46" s="12"/>
       <c r="AH46" s="11"/>
       <c r="AI46" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ46" s="11" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="AJ46" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK46" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL46" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="AN46" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO46" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP46" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5539,7 +6113,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E47" s="2" t="b">
         <v>0</v>
@@ -5548,7 +6122,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H47" s="2" t="b">
         <v>0</v>
@@ -5578,11 +6152,11 @@
         <v>0</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
@@ -5605,11 +6179,11 @@
         <v>0</v>
       </c>
       <c r="AB47" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE47" s="2"/>
       <c r="AF47" s="2"/>
@@ -5620,15 +6194,27 @@
         <v>0</v>
       </c>
       <c r="AI47" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ47" s="2" t="n">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AJ47" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK47" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AN47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP47" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5643,7 +6229,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E48" s="2" t="b">
         <v>0</v>
@@ -5652,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H48" s="2" t="b">
         <v>0</v>
@@ -5682,11 +6268,11 @@
         <v>0</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R48" s="2"/>
       <c r="S48" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
@@ -5709,26 +6295,38 @@
         <v>0</v>
       </c>
       <c r="AB48" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC48" s="2"/>
       <c r="AD48" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
       <c r="AG48" s="4"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ48" s="2" t="n">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AJ48" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK48" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM48" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AN48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP48" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5743,7 +6341,7 @@
         <v>3</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E49" s="11" t="b">
         <v>0</v>
@@ -5752,7 +6350,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H49" s="11" t="b">
         <v>0</v>
@@ -5782,11 +6380,11 @@
         <v>0</v>
       </c>
       <c r="Q49" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R49" s="11"/>
       <c r="S49" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T49" s="11"/>
       <c r="U49" s="11"/>
@@ -5809,26 +6407,38 @@
         <v>0</v>
       </c>
       <c r="AB49" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC49" s="11"/>
       <c r="AD49" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE49" s="11"/>
       <c r="AF49" s="11"/>
       <c r="AG49" s="12"/>
       <c r="AH49" s="11"/>
       <c r="AI49" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ49" s="11" t="n">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AJ49" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK49" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL49" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM49" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="AN49" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO49" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP49" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5843,7 +6453,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E50" s="2" t="b">
         <v>0</v>
@@ -5852,7 +6462,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H50" s="2" t="b">
         <v>0</v>
@@ -5882,11 +6492,11 @@
         <v>0</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R50" s="2"/>
       <c r="S50" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
@@ -5909,11 +6519,11 @@
         <v>0</v>
       </c>
       <c r="AB50" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
@@ -5924,15 +6534,27 @@
         <v>0</v>
       </c>
       <c r="AI50" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ50" s="2" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="AJ50" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM50" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="AN50" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP50" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5947,7 +6569,7 @@
         <v>2</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E51" s="2" t="b">
         <v>0</v>
@@ -5956,7 +6578,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H51" s="2" t="b">
         <v>0</v>
@@ -5986,11 +6608,11 @@
         <v>0</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R51" s="2"/>
       <c r="S51" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
@@ -6013,26 +6635,38 @@
         <v>0</v>
       </c>
       <c r="AB51" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC51" s="2"/>
       <c r="AD51" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE51" s="2"/>
       <c r="AF51" s="2"/>
       <c r="AG51" s="4"/>
       <c r="AH51" s="2"/>
       <c r="AI51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ51" s="2" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="AJ51" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK51" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM51" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="AN51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP51" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6047,7 +6681,7 @@
         <v>3</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E52" s="11" t="b">
         <v>0</v>
@@ -6056,7 +6690,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H52" s="11" t="b">
         <v>0</v>
@@ -6086,11 +6720,11 @@
         <v>0</v>
       </c>
       <c r="Q52" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R52" s="11"/>
       <c r="S52" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T52" s="11"/>
       <c r="U52" s="11"/>
@@ -6113,26 +6747,38 @@
         <v>0</v>
       </c>
       <c r="AB52" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC52" s="11"/>
       <c r="AD52" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE52" s="11"/>
       <c r="AF52" s="11"/>
       <c r="AG52" s="12"/>
       <c r="AH52" s="11"/>
       <c r="AI52" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ52" s="11" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="AJ52" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK52" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL52" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM52" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="AN52" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO52" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP52" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6147,7 +6793,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E53" s="2" t="b">
         <v>0</v>
@@ -6156,7 +6802,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H53" s="2" t="b">
         <v>0</v>
@@ -6186,11 +6832,11 @@
         <v>0</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R53" s="2"/>
       <c r="S53" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
@@ -6213,11 +6859,11 @@
         <v>0</v>
       </c>
       <c r="AB53" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC53" s="2"/>
       <c r="AD53" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE53" s="2"/>
       <c r="AF53" s="2"/>
@@ -6228,15 +6874,27 @@
         <v>0</v>
       </c>
       <c r="AI53" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ53" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="AJ53" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK53" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP53" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6251,7 +6909,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E54" s="2" t="b">
         <v>0</v>
@@ -6260,7 +6918,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H54" s="2" t="b">
         <v>0</v>
@@ -6290,11 +6948,11 @@
         <v>0</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
@@ -6317,26 +6975,38 @@
         <v>0</v>
       </c>
       <c r="AB54" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC54" s="2"/>
       <c r="AD54" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE54" s="2"/>
       <c r="AF54" s="2"/>
       <c r="AG54" s="4"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ54" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="AJ54" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK54" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM54" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN54" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP54" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6351,7 +7021,7 @@
         <v>3</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E55" s="11" t="b">
         <v>0</v>
@@ -6360,7 +7030,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H55" s="11" t="b">
         <v>0</v>
@@ -6390,11 +7060,11 @@
         <v>0</v>
       </c>
       <c r="Q55" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R55" s="11"/>
       <c r="S55" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T55" s="11"/>
       <c r="U55" s="11"/>
@@ -6417,26 +7087,38 @@
         <v>0</v>
       </c>
       <c r="AB55" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC55" s="11"/>
       <c r="AD55" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE55" s="11"/>
       <c r="AF55" s="11"/>
       <c r="AG55" s="12"/>
       <c r="AH55" s="11"/>
       <c r="AI55" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ55" s="11" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="AJ55" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK55" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL55" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM55" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN55" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO55" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP55" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6451,7 +7133,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E56" s="2" t="b">
         <v>0</v>
@@ -6460,7 +7142,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H56" s="2" t="b">
         <v>0</v>
@@ -6490,11 +7172,11 @@
         <v>0</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
@@ -6517,11 +7199,11 @@
         <v>0</v>
       </c>
       <c r="AB56" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AC56" s="2"/>
       <c r="AD56" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE56" s="2"/>
       <c r="AF56" s="2"/>
@@ -6532,15 +7214,27 @@
         <v>0</v>
       </c>
       <c r="AI56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ56" s="2" t="n">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="AJ56" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AK56" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM56" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="AN56" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP56" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6555,7 +7249,7 @@
         <v>2</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E57" s="2" t="b">
         <v>0</v>
@@ -6564,7 +7258,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H57" s="2" t="b">
         <v>0</v>
@@ -6594,11 +7288,11 @@
         <v>0</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
@@ -6621,26 +7315,38 @@
         <v>0</v>
       </c>
       <c r="AB57" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC57" s="2"/>
       <c r="AD57" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE57" s="2"/>
       <c r="AF57" s="2"/>
       <c r="AG57" s="4"/>
       <c r="AH57" s="2"/>
       <c r="AI57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ57" s="2" t="n">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="AJ57" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="AK57" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AL57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM57" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="AN57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP57" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6655,7 +7361,7 @@
         <v>3</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E58" s="11" t="b">
         <v>0</v>
@@ -6664,7 +7370,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H58" s="11" t="b">
         <v>0</v>
@@ -6694,11 +7400,11 @@
         <v>0</v>
       </c>
       <c r="Q58" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R58" s="11"/>
       <c r="S58" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T58" s="11"/>
       <c r="U58" s="11"/>
@@ -6721,26 +7427,38 @@
         <v>0</v>
       </c>
       <c r="AB58" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AC58" s="11"/>
       <c r="AD58" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE58" s="11"/>
       <c r="AF58" s="11"/>
       <c r="AG58" s="12"/>
       <c r="AH58" s="11"/>
       <c r="AI58" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ58" s="11" t="n">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="AJ58" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="AK58" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AL58" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM58" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="AN58" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO58" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP58" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6755,7 +7473,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E59" s="18" t="b">
         <v>0</v>
@@ -6764,7 +7482,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H59" s="18" t="b">
         <v>0</v>
@@ -6794,11 +7512,11 @@
         <v>0</v>
       </c>
       <c r="Q59" s="18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="R59" s="18"/>
       <c r="S59" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T59" s="18"/>
       <c r="U59" s="18"/>
@@ -6821,11 +7539,11 @@
         <v>0</v>
       </c>
       <c r="AB59" s="18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AC59" s="18"/>
       <c r="AD59" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE59" s="18"/>
       <c r="AF59" s="18"/>
@@ -6836,10 +7554,10 @@
         <v>1</v>
       </c>
       <c r="AI59" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ59" s="18" t="n">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="AJ59" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="AK59" s="18" t="n">
         <v>0</v>
@@ -6847,7 +7565,19 @@
       <c r="AL59" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="AM59" s="22"/>
+      <c r="AM59" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="AN59" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO59" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP59" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ59" s="22"/>
     </row>
     <row r="60">
       <c r="A60" s="18" t="n">
@@ -6860,7 +7590,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E60" s="18" t="b">
         <v>0</v>
@@ -6869,7 +7599,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H60" s="18" t="b">
         <v>0</v>
@@ -6899,11 +7629,11 @@
         <v>0</v>
       </c>
       <c r="Q60" s="18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="R60" s="18"/>
       <c r="S60" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T60" s="18"/>
       <c r="U60" s="18"/>
@@ -6926,21 +7656,21 @@
         <v>0</v>
       </c>
       <c r="AB60" s="18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AC60" s="18"/>
       <c r="AD60" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE60" s="18"/>
       <c r="AF60" s="18"/>
       <c r="AG60" s="19"/>
       <c r="AH60" s="18"/>
       <c r="AI60" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ60" s="18" t="n">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="AJ60" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="AK60" s="18" t="n">
         <v>0</v>
@@ -6948,7 +7678,19 @@
       <c r="AL60" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="AM60" s="22"/>
+      <c r="AM60" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="AN60" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO60" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP60" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ60" s="22"/>
     </row>
     <row r="61">
       <c r="A61" s="18" t="n">
@@ -6961,7 +7703,7 @@
         <v>3</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E61" s="18" t="b">
         <v>0</v>
@@ -6970,7 +7712,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H61" s="18" t="b">
         <v>0</v>
@@ -7000,11 +7742,11 @@
         <v>0</v>
       </c>
       <c r="Q61" s="18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="R61" s="18"/>
       <c r="S61" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T61" s="18"/>
       <c r="U61" s="18"/>
@@ -7027,21 +7769,21 @@
         <v>0</v>
       </c>
       <c r="AB61" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AC61" s="18"/>
       <c r="AD61" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AE61" s="18"/>
       <c r="AF61" s="18"/>
       <c r="AG61" s="19"/>
       <c r="AH61" s="18"/>
       <c r="AI61" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ61" s="18" t="n">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="AJ61" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="AK61" s="18" t="n">
         <v>0</v>
@@ -7049,10 +7791,22 @@
       <c r="AL61" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="AM61" s="22"/>
+      <c r="AM61" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="AN61" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO61" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP61" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ61" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL1"/>
+  <autoFilter ref="A1:AP1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>